<commit_message>
Selecionado Dados com loc()
</commit_message>
<xml_diff>
--- a/Arquivo.xlsx
+++ b/Arquivo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6813BFBD-0D2B-F249-9020-687C504B4EB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{527B6F05-7349-854D-9299-9D60787DCB99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Nome</t>
   </si>
@@ -38,6 +38,24 @@
   </si>
   <si>
     <t>Jonathan</t>
+  </si>
+  <si>
+    <t>Jessica</t>
+  </si>
+  <si>
+    <t>Amanda</t>
+  </si>
+  <si>
+    <t>Airton</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>Matheus</t>
+  </si>
+  <si>
+    <t>Maikon</t>
   </si>
 </sst>
 </file>
@@ -389,15 +407,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6809CD1-16BE-E742-AD40-63745429B697}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="9.28125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -422,6 +440,72 @@
         <v>10372926</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <v>92778477</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>62538263</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>54864244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>51127948</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>51818454</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>81842761</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>